<commit_message>
Resolved the first 5 childless-taxa found by 7a.qc_empty_taxa.sql. Backup: ICTVonline35.20200415.0106.step_7a_5of9_done.bak
</commit_message>
<xml_diff>
--- a/7a.qc_empty_taxa.sql.QC.xlsx
+++ b/7a.qc_empty_taxa.sql.QC.xlsx
@@ -553,7 +553,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,7 +699,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B5" t="s">
@@ -731,7 +731,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B6" t="s">

</xml_diff>

<commit_message>
complete step 7a: fix taxa with no children
</commit_message>
<xml_diff>
--- a/7a.qc_empty_taxa.sql.QC.xlsx
+++ b/7a.qc_empty_taxa.sql.QC.xlsx
@@ -104,58 +104,6 @@
     <t xml:space="preserve">phylum Cossaviricota created 3 times: sort=173, 177, 181. Will keep just the first. </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">sort=439 new family </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Redondoviridae</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> placed that family in root instead of in </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Recrevirales,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> as proposal had specified. </t>
-    </r>
-  </si>
-  <si>
-    <t>species "Escherichia phage vB_EcoS_NBD2" specified in proposal not created in spreadsheet. Will add as sort=1399.5</t>
-  </si>
-  <si>
     <t>split (sort=814.2) and create (sort=832) both create the genus, but in different places (realm:Riboviria, family: Rhabdoviridae, respectively)</t>
   </si>
   <si>
@@ -166,13 +114,19 @@
   </si>
   <si>
     <t>they forgot to abolish after moving out all sub-taxa; will abolish;  created sort=1849.5 for abolish action</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sort=439 new family Redondoviridae placed that family in root instead of in Recrevirales, as proposal had specified. </t>
+  </si>
+  <si>
+    <t>species"Escherichia virus NBD2", isolate "Escherichia phage vB_EcoS_NBD2" specified in proposal not created in spreadsheet. Will add as sort=1399.5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,19 +148,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -256,16 +197,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -553,7 +491,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,7 +510,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>11</v>
@@ -604,7 +542,7 @@
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -636,7 +574,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -668,7 +606,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -763,7 +701,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B7" t="s">
@@ -794,9 +732,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>26</v>
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
@@ -827,8 +765,8 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>27</v>
+      <c r="A9" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
@@ -860,7 +798,7 @@
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Found many isType issues (genera with 0 or >1 type species). Many issues come from past MSLs deleted extra reports, created MSL35 report.
</commit_message>
<xml_diff>
--- a/7a.qc_empty_taxa.sql.QC.xlsx
+++ b/7a.qc_empty_taxa.sql.QC.xlsx
@@ -104,9 +104,6 @@
     <t xml:space="preserve">phylum Cossaviricota created 3 times: sort=173, 177, 181. Will keep just the first. </t>
   </si>
   <si>
-    <t>split (sort=814.2) and create (sort=832) both create the genus, but in different places (realm:Riboviria, family: Rhabdoviridae, respectively)</t>
-  </si>
-  <si>
     <t>Fixes</t>
   </si>
   <si>
@@ -120,6 +117,9 @@
   </si>
   <si>
     <t>species"Escherichia virus NBD2", isolate "Escherichia phage vB_EcoS_NBD2" specified in proposal not created in spreadsheet. Will add as sort=1399.5</t>
+  </si>
+  <si>
+    <t>split (sort=814.2) and create (sort=832) both create the genus, but in different places (realm:Riboviria, family: Rhabdoviridae, respectively), IsWrong the create, and update the destintation for the split.</t>
   </si>
 </sst>
 </file>
@@ -491,7 +491,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,7 +510,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>11</v>
@@ -542,7 +542,7 @@
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -574,7 +574,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -606,7 +606,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -734,7 +734,7 @@
     </row>
     <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
@@ -766,7 +766,7 @@
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
@@ -797,8 +797,8 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>26</v>
+      <c r="A10" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>

</xml_diff>